<commit_message>
renaming files, making it more efficient
</commit_message>
<xml_diff>
--- a/outputs/final_features/spec_info.xlsx
+++ b/outputs/final_features/spec_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tinbuenafe/GitHub/PacificProj/outputs/final_features/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C252710-A8F9-F64A-A2FF-A431D9B28539}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{748D746E-132F-7A41-B8AA-07290A2D0355}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="15600" windowHeight="18780" xr2:uid="{7EBCD103-5E8B-4E4B-AA53-5E83CC4AB1FE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="15600" windowHeight="18680" xr2:uid="{7EBCD103-5E8B-4E4B-AA53-5E83CC4AB1FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="55">
   <si>
     <t>group</t>
   </si>
@@ -184,6 +184,21 @@
   </si>
   <si>
     <t>Rep-5414_surface</t>
+  </si>
+  <si>
+    <t>Caretta_caretta_IUCN</t>
+  </si>
+  <si>
+    <t>Chelonia_mydas_IUCN</t>
+  </si>
+  <si>
+    <t>Dermochelys_coriacea_IUCN</t>
+  </si>
+  <si>
+    <t>Eretmochelys_imbricata_IUCN</t>
+  </si>
+  <si>
+    <t>Lepidochelys_olivacea_IUCN</t>
   </si>
 </sst>
 </file>
@@ -535,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FBB5196-E5E5-E74E-9D99-1588CE6F2366}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -826,6 +841,106 @@
         <v>40</v>
       </c>
     </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>